<commit_message>
Updated fund information on submission
</commit_message>
<xml_diff>
--- a/Metabolomics_submission_07.03.2024/20240703_Metabolic profiling_Goldstein lab.xlsx
+++ b/Metabolomics_submission_07.03.2024/20240703_Metabolic profiling_Goldstein lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nunley17/Documents/Lab/Experiments/Experiments_2024/MYCN-IDH1-In-Vivo-experiments-03-22-2024/Metabolomics_submission_07.03.2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CCA419-3D0A-E247-9595-B161841CB556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63339D0F-5155-E94D-9656-EA4BFA73EDC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{DBD07577-1C69-B24D-B2AE-340B3FBC022B}"/>
+    <workbookView xWindow="31440" yWindow="2660" windowWidth="28800" windowHeight="16340" xr2:uid="{DBD07577-1C69-B24D-B2AE-340B3FBC022B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
   <si>
     <t>Date</t>
   </si>
@@ -65,24 +65,12 @@
     <t>Fund.Manager.Address</t>
   </si>
   <si>
-    <t>Box 951740, 22-215 CHS, Los Angeles, CA 90095-1740</t>
-  </si>
-  <si>
-    <t>SUND</t>
-  </si>
-  <si>
     <t>Vial Number</t>
   </si>
   <si>
     <t>Cell.Number</t>
   </si>
   <si>
-    <t>Emily Yu</t>
-  </si>
-  <si>
-    <t>EmilyYu@mednet.ucla.edu</t>
-  </si>
-  <si>
     <t>Human prostate</t>
   </si>
   <si>
@@ -92,9 +80,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>FUCRW</t>
-  </si>
-  <si>
     <t>MYCN</t>
   </si>
   <si>
@@ -165,6 +150,18 @@
   </si>
   <si>
     <t>IDH1-M2-1-C</t>
+  </si>
+  <si>
+    <t>RFP</t>
+  </si>
+  <si>
+    <t>N5WE</t>
+  </si>
+  <si>
+    <t>Kylin Sakamoto</t>
+  </si>
+  <si>
+    <t>kylin@lifesci.ucla.edu</t>
   </si>
 </sst>
 </file>
@@ -573,7 +570,7 @@
   <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +592,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -607,7 +604,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -640,35 +637,32 @@
         <v>45476</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="I2" s="4"/>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -679,22 +673,22 @@
         <v>45476</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="7" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="I3" s="4"/>
     </row>
@@ -706,22 +700,22 @@
         <v>45476</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I4" s="4"/>
     </row>
@@ -733,22 +727,22 @@
         <v>45476</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I5" s="4"/>
     </row>
@@ -760,22 +754,22 @@
         <v>45476</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>22</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>27</v>
       </c>
       <c r="I6" s="4"/>
     </row>
@@ -787,22 +781,22 @@
         <v>45476</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="I7" s="4"/>
     </row>
@@ -814,22 +808,22 @@
         <v>45476</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I8" s="4"/>
     </row>
@@ -841,22 +835,22 @@
         <v>45476</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -868,22 +862,22 @@
         <v>45476</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I10" s="4"/>
     </row>
@@ -895,22 +889,22 @@
         <v>45476</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I11" s="4"/>
     </row>
@@ -922,22 +916,22 @@
         <v>45476</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I12" s="4"/>
     </row>
@@ -949,22 +943,22 @@
         <v>45476</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I13" s="4"/>
     </row>
@@ -976,22 +970,22 @@
         <v>45476</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
@@ -1002,22 +996,22 @@
         <v>45476</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
@@ -1028,22 +1022,22 @@
         <v>45476</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1054,22 +1048,22 @@
         <v>45476</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1080,22 +1074,22 @@
         <v>45476</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1106,22 +1100,22 @@
         <v>45476</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1132,22 +1126,22 @@
         <v>45476</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1158,22 +1152,22 @@
         <v>45476</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1184,22 +1178,22 @@
         <v>45476</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1376,7 +1370,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" display="mailto:EmilyYu@mednet.ucla.edu" xr:uid="{1D8C5343-3465-694F-98D7-5821CAC1C39D}"/>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{1D8C5343-3465-694F-98D7-5821CAC1C39D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>